<commit_message>
New file is added
</commit_message>
<xml_diff>
--- a/Xray_Performance_Analysis.xlsx
+++ b/Xray_Performance_Analysis.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Meeravali_Workspace\Cypress\Cypress\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{195F19E1-05A0-4634-85D3-FE79F7B1BA89}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDB721DD-3F95-42B3-A637-0FCB28F344CA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -243,7 +243,7 @@
 - Sending report to stakeholder</t>
   </si>
   <si>
-    <t>TestFile</t>
+    <t>TestFile me one two three</t>
   </si>
 </sst>
 </file>

</xml_diff>